<commit_message>
add test cases of AuthForRestfulReadTests and AuthForWebserviceTests
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.10.0.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1053136A-4FAB-4FF3-B209-D20155628E35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D28B37-F44E-4440-8449-0977A958790B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
+    <sheet name="authForRestfulRead" sheetId="3" r:id="rId2"/>
+    <sheet name="authForWebserviceRead" sheetId="4" r:id="rId3"/>
+    <sheet name="authForWebserviceWrite" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="146">
   <si>
     <t>name</t>
   </si>
@@ -277,12 +280,338 @@
   </si>
   <si>
     <t>not exist in entity!</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-1</t>
+  </si>
+  <si>
+    <t>authInfo</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"basic",
+        "dataSourceName":"UserReadWithBasicAuth",
+        "detail":{
+            "value":"name=admin pwd=123456"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>UserReadWithBasicAuth</t>
+  </si>
+  <si>
+    <t>106103</t>
+  </si>
+  <si>
+    <t>sql execution failed</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-2</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-3</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+(authType:basic)</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is NONE
+(authType:basic)</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is wrong
+(authType:basic)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"basic",
+        "dataSourceName":"UserReadWithBasicAuth",
+        "detail":{
+            "value":"name=admin pwd=123457"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-4</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-5</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-6</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-7</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-8</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-9</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-10</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-11</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-12</t>
+  </si>
+  <si>
+    <t>UserReadWithOauthAuth</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"OAUTH",
+        "dataSourceName":"UserReadWithOauthAuth",
+        "detail":{
+            "value":"admin123456"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+(authType:OAUTH)</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is NONE
+(authType:OAUTH)</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is wrong
+(authType:OAUTH)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"OAUTH",
+        "dataSourceName":"UserReadWithOauthAuth",
+        "detail":{
+            "value":"admin123457"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"Cookie",
+        "dataSourceName":"UserReadWithCookieAuth",
+        "detail":{
+            "value":"key1=value1;key2=value2"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+(authType:Cookie)</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is NONE
+(authType:Cookie)</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is wrong
+(authType:Cookie)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"Cookie",
+        "dataSourceName":"UserReadWithCookieAuth",
+        "detail":{
+            "value":"key1=value1;key2=value3"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>UserReadWithCookieAuth</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+(authType:TOKEN)</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is NONE
+(authType:TOKEN)</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is wrong
+(authType:TOKEN)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"TOKEN",
+        "dataSourceName":"UserReadWithTokenAuth",
+        "detail":{
+            "value":"admin123456"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"TOKEN",
+        "dataSourceName":"UserReadWithTokenAuth",
+        "detail":{
+            "value":"admin123457"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>UserReadWithTokenAuth</t>
+  </si>
+  <si>
+    <t>jinzu-webservice-read-auth-test-1</t>
+  </si>
+  <si>
+    <t>jinzu-webservice-read-auth-test-2</t>
+  </si>
+  <si>
+    <t>jinzu-webservice-read-auth-test-3</t>
+  </si>
+  <si>
+    <t>warehouse</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"SoapHeaderAuth",
+        "dataSourceName":"ws_hdl_datasource",
+        "detail":{
+            "value":"key2=value2"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"SoapHeaderAuth",
+        "dataSourceName":"ws_hdl_datasource",
+        "detail":{
+            "value":"key2=value3"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+(authType:SoapHeaderAuth)</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is NONE
+(authType:SoapHeaderAuth)</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is wrong
+(authType:SoapHeaderAuth)</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Operate success.</t>
+  </si>
+  <si>
+    <t>rspData</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {
+      "number": "1111",
+      "id": "1111",
+      "message": "5555",
+      "type": "55551"
+    }
+    {
+      "number": "2222",
+      "id": "2222",
+      "message": "6666",
+      "type": "6666"
+    }</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>jinzu-webservice-write-auth-test-1</t>
+  </si>
+  <si>
+    <t>jinzu-webservice-write-auth-test-2</t>
+  </si>
+  <si>
+    <t>jinzu-webservice-write-auth-test-3</t>
+  </si>
+  <si>
+    <t>insertInfo</t>
+  </si>
+  <si>
+    <t>{
+    "warehousewrite":[
+        {
+            "stockItem":[
+                {
+                    "WMS_GUID":"10016",
+                    "BUDAT":"t5"
+                },
+                {
+                    "WMS_GUID":"10016",
+                    "BUDAT":"t7"
+                }
+            ]
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+            "number": null,
+            "id": null,
+            "message": null,
+            "type": null
+          }</t>
+  </si>
+  <si>
+    <t>{
+            "number": "1111",
+            "id": "5555",
+            "message": "1111",
+            "type": "55551"
+          }
+          {
+            "number": "2222",
+            "id": "6666",
+            "message": "2222",
+            "type": "6666"
+          }</t>
+  </si>
+  <si>
+    <t>entityName</t>
+  </si>
+  <si>
+    <t>warehousewrite</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -346,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -354,6 +683,30 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,15 +989,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M20" sqref="M20"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="12.6328125" style="1"/>
+    <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -1776,4 +2129,535 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{290FAA0B-7149-479D-BD5C-41CB62B5D856}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="12.6640625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9AA3231-45F1-4093-9E13-DF6B3255B3C5}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="12.6640625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="165.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D36F244A-FF43-4D07-8FA4-A5F42AB30D28}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="12.6640625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modify test cases if jinzu entitymanagement
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-with-comment\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC4A02A-7DAA-46EF-9EDF-F21440D7B988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF08606-CA75-4213-8990-0EE92A43BD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-14570" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="147">
   <si>
     <t>name</t>
   </si>
@@ -582,28 +582,45 @@
           }</t>
   </si>
   <si>
+    <t>entityName</t>
+  </si>
+  <si>
+    <t>warehousewrite</t>
+  </si>
+  <si>
+    <t>This entity 12321 is not found in domain</t>
+  </si>
+  <si>
     <t>{
-            "number": "1111",
+    "warehousewrite": [
+        {
+            "stockItem": [
+                {
+                    "WMS_GUID": "10016",
+                    "BUDAT": "t5"
+                },
+                {
+                    "WMS_GUID": "10016",
+                    "BUDAT": "t7"
+                }
+            ]
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+            "number": "1",
             "id": "5555",
-            "message": "1111",
-            "type": "55551"
-          }
-          {
-            "number": "2222",
-            "id": "6666",
-            "message": "2222",
-            "type": "6666"
-          }</t>
-  </si>
-  <si>
-    <t>entityName</t>
-  </si>
-  <si>
-    <t>warehousewrite</t>
-  </si>
-  <si>
-    <t>[add domain entities for mapping success] info</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+            "type": "1",
+            "message": "5555"
+        }
+        {
+            "number": "3",
+            "id": "3333",
+            "type": "3",
+            "message": "3333"
+        }</t>
   </si>
 </sst>
 </file>
@@ -617,20 +634,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -990,12 +1007,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
+      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
     <col min="3" max="12" width="12.6640625" style="1"/>
@@ -1003,7 +1020,7 @@
     <col min="14" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1044,7 +1061,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -1065,7 +1082,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -1086,7 +1103,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
@@ -1113,7 +1130,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
@@ -1132,13 +1149,13 @@
       <c r="J5" s="3"/>
       <c r="K5" s="4"/>
       <c r="L5" s="3">
-        <v>106920</v>
+        <v>108002</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -1161,7 +1178,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>42</v>
       </c>
@@ -1184,7 +1201,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>43</v>
       </c>
@@ -1207,7 +1224,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>44</v>
       </c>
@@ -1230,7 +1247,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>45</v>
       </c>
@@ -1253,7 +1270,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>46</v>
       </c>
@@ -1276,7 +1293,7 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>47</v>
       </c>
@@ -1299,7 +1316,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>48</v>
       </c>
@@ -1322,7 +1339,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>49</v>
       </c>
@@ -1345,7 +1362,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>50</v>
       </c>
@@ -1368,7 +1385,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>51</v>
       </c>
@@ -1391,7 +1408,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>52</v>
       </c>
@@ -1418,7 +1435,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>53</v>
       </c>
@@ -1445,7 +1462,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>54</v>
       </c>
@@ -1468,7 +1485,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>55</v>
       </c>
@@ -1493,7 +1510,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>56</v>
       </c>
@@ -1518,7 +1535,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>57</v>
       </c>
@@ -1543,7 +1560,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>58</v>
       </c>
@@ -1570,7 +1587,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>59</v>
       </c>
@@ -1597,7 +1614,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>60</v>
       </c>
@@ -1624,7 +1641,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>61</v>
       </c>
@@ -1651,7 +1668,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>62</v>
       </c>
@@ -1674,7 +1691,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>63</v>
       </c>
@@ -1697,7 +1714,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>64</v>
       </c>
@@ -1720,7 +1737,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>65</v>
       </c>
@@ -1743,7 +1760,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>66</v>
       </c>
@@ -1768,7 +1785,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>67</v>
       </c>
@@ -1793,7 +1810,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>68</v>
       </c>
@@ -1818,7 +1835,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>69</v>
       </c>
@@ -1843,7 +1860,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>70</v>
       </c>
@@ -1868,7 +1885,7 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>71</v>
       </c>
@@ -1893,7 +1910,7 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>72</v>
       </c>
@@ -1918,7 +1935,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>73</v>
       </c>
@@ -1943,7 +1960,7 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>74</v>
       </c>
@@ -1966,7 +1983,7 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>75</v>
       </c>
@@ -1989,7 +2006,7 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>76</v>
       </c>
@@ -2012,7 +2029,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>77</v>
       </c>
@@ -2035,7 +2052,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>78</v>
       </c>
@@ -2058,7 +2075,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>79</v>
       </c>
@@ -2081,7 +2098,7 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>80</v>
       </c>
@@ -2104,7 +2121,7 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>81</v>
       </c>
@@ -2142,7 +2159,7 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.21875" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="9" bestFit="1" customWidth="1"/>
@@ -2154,7 +2171,7 @@
     <col min="8" max="16384" width="12.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
@@ -2177,7 +2194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="132" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>83</v>
       </c>
@@ -2194,7 +2211,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>89</v>
       </c>
@@ -2213,7 +2230,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="132" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>90</v>
       </c>
@@ -2234,7 +2251,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="132" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="138" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>95</v>
       </c>
@@ -2251,7 +2268,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>96</v>
       </c>
@@ -2270,7 +2287,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="132" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="138" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>97</v>
       </c>
@@ -2291,7 +2308,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="132" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="138" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>98</v>
       </c>
@@ -2308,7 +2325,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>99</v>
       </c>
@@ -2327,7 +2344,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="132" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="138" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>100</v>
       </c>
@@ -2348,7 +2365,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="132" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="138" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>101</v>
       </c>
@@ -2365,7 +2382,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>102</v>
       </c>
@@ -2384,7 +2401,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="132" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="138" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>103</v>
       </c>
@@ -2420,9 +2437,9 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.88671875" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" style="9" bestFit="1" customWidth="1"/>
@@ -2433,7 +2450,7 @@
     <col min="9" max="16384" width="12.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
@@ -2459,7 +2476,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="184.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>122</v>
       </c>
@@ -2479,7 +2496,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>123</v>
       </c>
@@ -2501,7 +2518,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="132" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>124</v>
       </c>
@@ -2536,25 +2553,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D36F244A-FF43-4D07-8FA4-A5F42AB30D28}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5546875" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.44140625" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.33203125" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="12.6640625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
@@ -2565,7 +2582,7 @@
         <v>84</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>139</v>
@@ -2583,7 +2600,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="237.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>136</v>
       </c>
@@ -2594,19 +2611,19 @@
         <v>126</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="14"/>
       <c r="H2" s="13"/>
       <c r="I2" s="13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="237.6" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>137</v>
       </c>
@@ -2615,7 +2632,7 @@
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>140</v>
@@ -2631,7 +2648,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="237.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>138</v>
       </c>
@@ -2642,7 +2659,7 @@
         <v>127</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>140</v>

</xml_diff>

<commit_message>
add query Invert entity for multi datsources join
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-backup\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBF696B-9B8C-4F36-AA20-7427A6D93B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E2529D-B504-4FE4-BF4E-8D3BA1E06597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-14570" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="161">
   <si>
     <t>name</t>
   </si>
@@ -664,6 +664,21 @@
   </si>
   <si>
     <t>condition</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>jinzu-connector-test-8-var23</t>
+  </si>
+  <si>
+    <t>good request, data retrieved</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inverter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>good request, data retrieved,no schema check</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1049,11 +1064,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2131,7 +2146,7 @@
         <v>77</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>4</v>
+        <v>158</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -2227,6 +2242,17 @@
       </c>
       <c r="N48" s="1" t="s">
         <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update EnlightedSensorDetails case due to device issue
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFA1FB2-6781-4D7E-AC39-0E572A74B2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD914A67-B066-4136-8DC6-C16EF3057EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1392" windowWidth="21960" windowHeight="12408" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -633,14 +633,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>floor_id='1' and from_date='202203071530' and to_date='202203071537'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>floor_id='1' and from_date='202203071530' and to_date='202203071540'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>jinzu-connector-test-8-var22</t>
   </si>
   <si>
@@ -664,6 +656,14 @@
   </si>
   <si>
     <t>condition</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>floor_id='1' and from_date='202205221500' and to_date='202205221537'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>floor_id='1' and from_date='202205221527' and to_date='202205221537'</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -678,20 +678,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1051,12 +1051,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="38.77734375" style="1" customWidth="1"/>
@@ -1068,7 +1068,7 @@
     <col min="14" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>8</v>
@@ -1109,10 +1109,10 @@
         <v>14</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -1133,7 +1133,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1154,7 +1154,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
@@ -1229,7 +1229,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>40</v>
       </c>
@@ -1252,7 +1252,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>41</v>
       </c>
@@ -1275,7 +1275,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>42</v>
       </c>
@@ -1298,7 +1298,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>43</v>
       </c>
@@ -1321,7 +1321,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>44</v>
       </c>
@@ -1344,7 +1344,7 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>45</v>
       </c>
@@ -1367,7 +1367,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>46</v>
       </c>
@@ -1390,7 +1390,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>47</v>
       </c>
@@ -1413,7 +1413,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>48</v>
       </c>
@@ -1436,7 +1436,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>49</v>
       </c>
@@ -1459,7 +1459,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>50</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>51</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>52</v>
       </c>
@@ -1536,7 +1536,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>53</v>
       </c>
@@ -1561,7 +1561,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>54</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>55</v>
       </c>
@@ -1611,7 +1611,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>56</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>57</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>58</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>59</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>60</v>
       </c>
@@ -1742,7 +1742,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>61</v>
       </c>
@@ -1765,7 +1765,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>62</v>
       </c>
@@ -1788,7 +1788,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>63</v>
       </c>
@@ -1811,7 +1811,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>64</v>
       </c>
@@ -1836,7 +1836,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>65</v>
       </c>
@@ -1861,7 +1861,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>66</v>
       </c>
@@ -1886,7 +1886,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>67</v>
       </c>
@@ -1911,7 +1911,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>68</v>
       </c>
@@ -1936,7 +1936,7 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>69</v>
       </c>
@@ -1961,7 +1961,7 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>70</v>
       </c>
@@ -1986,7 +1986,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>71</v>
       </c>
@@ -2011,7 +2011,7 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>72</v>
       </c>
@@ -2034,7 +2034,7 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>73</v>
       </c>
@@ -2057,7 +2057,7 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>74</v>
       </c>
@@ -2080,7 +2080,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>75</v>
       </c>
@@ -2103,7 +2103,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>76</v>
       </c>
@@ -2126,7 +2126,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>77</v>
       </c>
@@ -2149,7 +2149,7 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>78</v>
       </c>
@@ -2172,7 +2172,7 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>79</v>
       </c>
@@ -2195,38 +2195,38 @@
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>147</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="N47" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C47" s="1" t="s">
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="N47" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="C48" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="N48" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2240,11 +2240,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{290FAA0B-7149-479D-BD5C-41CB62B5D856}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.21875" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="9" bestFit="1" customWidth="1"/>
@@ -2256,7 +2256,7 @@
     <col min="8" max="16384" width="12.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>81</v>
       </c>
@@ -2296,7 +2296,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>87</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>88</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>93</v>
       </c>
@@ -2353,7 +2353,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>94</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>95</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>96</v>
       </c>
@@ -2410,7 +2410,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>97</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>98</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>99</v>
       </c>
@@ -2467,7 +2467,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>100</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>101</v>
       </c>
@@ -2522,7 +2522,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.88671875" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="9" bestFit="1" customWidth="1"/>
@@ -2535,7 +2535,7 @@
     <col min="9" max="16384" width="12.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="184.8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>120</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>121</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="132" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>122</v>
       </c>
@@ -2642,7 +2642,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5546875" style="12" bestFit="1" customWidth="1"/>
@@ -2656,7 +2656,7 @@
     <col min="10" max="16384" width="12.6640625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="237.6" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>133</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="237.6" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>134</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="237.6" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>135</v>
       </c>

</xml_diff>

<commit_message>
update for EnlightedSensorDetails query becasue of data loss and change condition
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E19E612-AAF5-41E8-8484-F5488FD5BDF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D5318F-C2D6-41B6-A5FA-07F383C34399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-14560" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -123,9 +123,6 @@
     <t>jinzu-connector-test-3-var1</t>
   </si>
   <si>
-    <t>LEASE_NO='V000000030' AND location='海南省儋州市'</t>
-  </si>
-  <si>
     <t>city='儋州市'</t>
   </si>
   <si>
@@ -645,14 +642,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>floor_id='1' and from_date='202205221500' and to_date='202205221537'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>floor_id='1' and from_date='202205221527' and to_date='202205221537'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>{
     "number": "1",
     "id": "5555",
@@ -666,6 +655,18 @@
     "message": "3"
 }</t>
   </si>
+  <si>
+    <t>id='V000000030' AND location='海南省儋州市'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>floor_id='1' and from_date='202207221527' and to_date='202207221537'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>floor_id='1' and from_date='202207221500' and to_date='202207221537'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -678,20 +679,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1051,12 +1052,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="38.77734375" style="1" customWidth="1"/>
@@ -1068,7 +1069,7 @@
     <col min="14" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1076,7 +1077,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>8</v>
@@ -1109,10 +1110,10 @@
         <v>14</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -1133,7 +1134,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1154,7 +1155,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -1181,7 +1182,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -1203,10 +1204,10 @@
         <v>108002</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
@@ -1214,7 +1215,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -1229,15 +1230,15 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>31</v>
+        <v>154</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1252,15 +1253,15 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1275,15 +1276,15 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1298,9 +1299,9 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
@@ -1321,9 +1322,9 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
@@ -1344,9 +1345,9 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>18</v>
@@ -1367,9 +1368,9 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>18</v>
@@ -1390,9 +1391,9 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>4</v>
@@ -1400,7 +1401,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>25</v>
@@ -1413,9 +1414,9 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>4</v>
@@ -1423,7 +1424,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>25</v>
@@ -1436,9 +1437,9 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>4</v>
@@ -1459,9 +1460,9 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>21</v>
@@ -1483,12 +1484,12 @@
         <v>106107</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>21</v>
@@ -1496,7 +1497,7 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>25</v>
@@ -1510,12 +1511,12 @@
         <v>106107</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>4</v>
@@ -1527,7 +1528,7 @@
         <v>25</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -1536,9 +1537,9 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>4</v>
@@ -1550,7 +1551,7 @@
         <v>25</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3">
@@ -1561,9 +1562,9 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>4</v>
@@ -1575,7 +1576,7 @@
         <v>25</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3">
@@ -1586,9 +1587,9 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>4</v>
@@ -1600,7 +1601,7 @@
         <v>25</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3">
@@ -1611,9 +1612,9 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>22</v>
@@ -1635,12 +1636,12 @@
         <v>106107</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>22</v>
@@ -1662,12 +1663,12 @@
         <v>106107</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>22</v>
@@ -1689,12 +1690,12 @@
         <v>106107</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>22</v>
@@ -1716,12 +1717,12 @@
         <v>106107</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>4</v>
@@ -1742,9 +1743,9 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>4</v>
@@ -1765,9 +1766,9 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>4</v>
@@ -1788,9 +1789,9 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>4</v>
@@ -1811,9 +1812,9 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>4</v>
@@ -1836,9 +1837,9 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>4</v>
@@ -1861,9 +1862,9 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>4</v>
@@ -1886,9 +1887,9 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>4</v>
@@ -1911,9 +1912,9 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>4</v>
@@ -1936,9 +1937,9 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>4</v>
@@ -1961,9 +1962,9 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>4</v>
@@ -1986,9 +1987,9 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>4</v>
@@ -2011,9 +2012,9 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>4</v>
@@ -2034,9 +2035,9 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>4</v>
@@ -2057,9 +2058,9 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>4</v>
@@ -2080,9 +2081,9 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>4</v>
@@ -2103,9 +2104,9 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>4</v>
@@ -2126,9 +2127,9 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>4</v>
@@ -2149,9 +2150,9 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>4</v>
@@ -2172,9 +2173,9 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>4</v>
@@ -2195,38 +2196,38 @@
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F47" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="N47" s="1" t="s">
+      <c r="C48" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="N48" s="1" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="N48" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2244,7 +2245,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.21875" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="9" bestFit="1" customWidth="1"/>
@@ -2256,7 +2257,7 @@
     <col min="8" max="16384" width="12.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
@@ -2264,7 +2265,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>0</v>
@@ -2279,232 +2280,232 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="D4" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="D7" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>112</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>119</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2522,7 +2523,7 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.88671875" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="9" bestFit="1" customWidth="1"/>
@@ -2535,7 +2536,7 @@
     <col min="9" max="16384" width="12.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
@@ -2543,7 +2544,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>0</v>
@@ -2558,73 +2559,73 @@
         <v>14</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="165.6" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="158.4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="10"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>130</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="124.2" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="132" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>122</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>123</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>130</v>
-      </c>
       <c r="H4" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2638,11 +2639,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D36F244A-FF43-4D07-8FA4-A5F42AB30D28}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5546875" style="12" bestFit="1" customWidth="1"/>
@@ -2656,7 +2657,7 @@
     <col min="10" max="16384" width="12.6640625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
@@ -2664,13 +2665,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>13</v>
@@ -2682,82 +2683,82 @@
         <v>14</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="237.6" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="14"/>
       <c r="H2" s="13"/>
       <c r="I2" s="13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="237.6" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>130</v>
-      </c>
       <c r="I3" s="13" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="237.6" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="H4" s="13" t="s">
-        <v>130</v>
-      </c>
       <c r="I4" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add case for connector cache
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D5318F-C2D6-41B6-A5FA-07F383C34399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586AC1F3-925A-4990-9C17-6C9CE57810DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-14560" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24720" yWindow="-10280" windowWidth="28800" windowHeight="15500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
     <sheet name="authForRestfulRead" sheetId="3" r:id="rId2"/>
     <sheet name="authForWebserviceRead" sheetId="4" r:id="rId3"/>
     <sheet name="authForWebserviceWrite" sheetId="5" r:id="rId4"/>
+    <sheet name="getAllCacheNames" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="161">
   <si>
     <t>name</t>
   </si>
@@ -667,6 +668,22 @@
     <t>floor_id='1' and from_date='202207221500' and to_date='202207221537'</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>jinzu-connector-cache-test1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>get allCacheNames</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dataList</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>table_schema,datasource_config,datasource_restTemplate,datasource_connection,mapper,datasource_auth,datasource_freemarker,datasource_webservice,executorBaseInfo,plugin_relatedDb,plugin_thriftClient,plugin_debug,entityCache,data,meta,rule</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -675,7 +692,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -694,6 +711,13 @@
       <sz val="8"/>
       <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1052,9 +1076,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2766,4 +2790,55 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8601E93B-0ADC-4830-874C-EAC42F02D192}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.77734375" customWidth="1"/>
+    <col min="2" max="3" width="26.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add new case of connector cache
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586AC1F3-925A-4990-9C17-6C9CE57810DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4F57E2-6D93-4043-863E-6E5D68D09183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24720" yWindow="-10280" windowWidth="28800" windowHeight="15500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2088" yWindow="3288" windowWidth="19764" windowHeight="10044" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="authForWebserviceRead" sheetId="4" r:id="rId3"/>
     <sheet name="authForWebserviceWrite" sheetId="5" r:id="rId4"/>
     <sheet name="getAllCacheNames" sheetId="6" r:id="rId5"/>
+    <sheet name="getCacheKeyAndValue" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="171">
   <si>
     <t>name</t>
   </si>
@@ -682,6 +683,45 @@
   </si>
   <si>
     <t>table_schema,datasource_config,datasource_restTemplate,datasource_connection,mapper,datasource_auth,datasource_freemarker,datasource_webservice,executorBaseInfo,plugin_relatedDb,plugin_thriftClient,plugin_debug,entityCache,data,meta,rule</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>jinzu-connector-cache-test2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>entityName</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Site</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>cacheName</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>jinzu-connector-cache-test3</t>
+  </si>
+  <si>
+    <t>Inverter</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>datasource_auth</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> data,check get cache key and value</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>datasource_auth,check get cache key and value</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2796,8 +2836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8601E93B-0ADC-4830-874C-EAC42F02D192}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2841,4 +2881,78 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF5B3EA0-A528-4027-A2D0-5115649CB22B}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5546875" customWidth="1"/>
+    <col min="2" max="2" width="45.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27.21875" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix sdl-10000 update case
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4F57E2-6D93-4043-863E-6E5D68D09183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CA10CC-D009-4DF7-AC64-06ACAAC0ABE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2088" yWindow="3288" windowWidth="19764" windowHeight="10044" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -662,14 +662,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>floor_id='1' and from_date='202207221527' and to_date='202207221537'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>floor_id='1' and from_date='202207221500' and to_date='202207221537'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>jinzu-connector-cache-test1</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -723,6 +715,14 @@
   <si>
     <t>datasource_auth,check get cache key and value</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>floor_id='1' and from_date='202209221527' and to_date='202209221537'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>floor_id='1' and from_date='202209221527' and to_date='202209221530'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1116,9 +1116,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2268,7 +2268,7 @@
         <v>148</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>147</v>
@@ -2285,7 +2285,7 @@
         <v>148</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>147</v>
@@ -2854,7 +2854,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
@@ -2868,13 +2868,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" t="s">
         <v>158</v>
-      </c>
-      <c r="C2" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2887,7 +2887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF5B3EA0-A528-4027-A2D0-5115649CB22B}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2907,10 +2907,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>13</v>
@@ -2924,30 +2924,30 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" t="s">
         <v>161</v>
-      </c>
-      <c r="B2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" t="s">
         <v>166</v>
       </c>
-      <c r="B3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C3" t="s">
-        <v>168</v>
-      </c>
       <c r="D3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Modbus test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CA10CC-D009-4DF7-AC64-06ACAAC0ABE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB178E3-62DD-4717-B55F-E79CF0EE33AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="authForWebserviceWrite" sheetId="5" r:id="rId4"/>
     <sheet name="getAllCacheNames" sheetId="6" r:id="rId5"/>
     <sheet name="getCacheKeyAndValue" sheetId="7" r:id="rId6"/>
+    <sheet name="queryModbusEntity" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="174">
   <si>
     <t>name</t>
   </si>
@@ -723,6 +724,18 @@
   <si>
     <t>floor_id='1' and from_date='202209221527' and to_date='202209221530'</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>jinzu-modbus-query-var1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stime &gt; '$start_time' and stime &lt;  '$end_time'</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ModbusTestEntity</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1116,9 +1129,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2955,4 +2968,93 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE978BC4-4288-4EAE-BF7E-ADEDA14A16D0}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="62.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.77734375" customWidth="1"/>
+    <col min="8" max="8" width="24.88671875" customWidth="1"/>
+    <col min="13" max="13" width="22.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add realtime persistence case
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-connector-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB178E3-62DD-4717-B55F-E79CF0EE33AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71A3341-957C-47FE-8037-7EBFC6AB1E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="getAllCacheNames" sheetId="6" r:id="rId5"/>
     <sheet name="getCacheKeyAndValue" sheetId="7" r:id="rId6"/>
     <sheet name="queryModbusEntity" sheetId="8" r:id="rId7"/>
+    <sheet name="checkRealtimePersistence" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="180">
   <si>
     <t>name</t>
   </si>
@@ -737,6 +738,38 @@
     <t>ModbusTestEntity</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>sql</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>truncate table chdb.Event_local on cluster clickhouse</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>entityName</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Event</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[
+    {
+      "eventTag": "success",
+      "coilNum": "1",
+      "device": "device1",
+      "processNum": "realtime persistence verify",
+      "timestamp": "2023-1-1"
+    }
+  ]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>expectedResponseData</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -745,7 +778,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -772,6 +805,11 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -815,7 +853,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -846,6 +884,12 @@
     </xf>
     <xf numFmtId="12" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1129,7 +1173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD3"/>
     </sheetView>
@@ -3057,4 +3101,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37936975-B808-4589-906A-809ED9C9B6DD}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.77734375" customWidth="1"/>
+    <col min="2" max="2" width="31.21875" customWidth="1"/>
+    <col min="3" max="3" width="37.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="138" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>